<commit_message>
Bilevel_Optim workflow in progress
</commit_message>
<xml_diff>
--- a/docu/TestExperimentSet1/TestExperiment1.xlsx
+++ b/docu/TestExperimentSet1/TestExperiment1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216A5384-FA47-4F15-8B93-C6060BF9D2CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13359581-D238-4235-88D7-6E25739C5D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13530" yWindow="2970" windowWidth="14850" windowHeight="12045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11115" yWindow="1830" windowWidth="16155" windowHeight="12510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1006,7 +1006,7 @@
   <dimension ref="A1:N47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:L47"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1028,7 +1028,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>235</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -1042,7 +1042,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>

</xml_diff>